<commit_message>
update ui spec template
</commit_message>
<xml_diff>
--- a/myproject/media/login_template.xlsx
+++ b/myproject/media/login_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -516,12 +516,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Khi người dùng đăng nhập</t>
+          <t>Không chứa ký tự đặc biệt</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Tên người dùng hợp lệ</t>
+          <t>"user123"</t>
         </is>
       </c>
     </row>
@@ -548,22 +548,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Khi người dùng đăng nhập</t>
+          <t>Phải có ít nhất 1 ký tự số và 1 ký tự đặc biệt</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Mật khẩu hợp lệ</t>
+          <t>"P@ssw0rd!"</t>
         </is>
       </c>
     </row>
@@ -600,12 +600,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Khi người dùng chọn</t>
+          <t>Chọn nếu muốn lưu mật khẩu trên trình duyệt</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Lưu thông tin đăng nhập</t>
+          <t>true/false</t>
         </is>
       </c>
     </row>
@@ -617,17 +617,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Quên mật khẩu</t>
+          <t>Đăng nhập</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Không</t>
+          <t>Có</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Link</t>
+          <t>Button</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -642,12 +642,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Khi người dùng click</t>
+          <t>Click để xác thực thông tin đăng nhập</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Điều hướng sang trang quên mật khẩu</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -659,17 +659,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Đăng nhập</t>
+          <t>Quên mật khẩu</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Có</t>
+          <t>Không</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Button</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -684,12 +684,54 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Khi người dùng nhấn</t>
+          <t>Chuyển đến trang khôi phục mật khẩu</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Gửi thông tin đăng nhập</t>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Đăng ký tài khoản</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Chuyển đến trang đăng ký tài khoản</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>